<commit_message>
Correzione file Excel su richiesta del team FSE 2.0
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CAVALLAROXX/CAVALLARO_GIUSEPPE/AUTOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CAVALLAROXX/CAVALLARO_GIUSEPPE/AUTOFSE/1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="202">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1662,7 +1662,7 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1677,32 +1677,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="285.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1715,12 +1715,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1749,7 +1749,7 @@
   </sheetPr>
   <dimension ref="A1:B996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -2826,12 +2826,12 @@
   </sheetPr>
   <dimension ref="A1:W1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H18" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="O19" activeCellId="0" sqref="O19"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3047,7 +3047,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="15"/>
     </row>
-    <row r="9" s="26" customFormat="true" ht="72.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="26" customFormat="true" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="n">
         <v>32</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="n">
         <v>40</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="n">
         <v>48</v>
       </c>
@@ -3260,11 +3260,17 @@
       <c r="E12" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="F12" s="30" t="n">
+        <v>45817</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>62</v>
+      </c>
       <c r="H12" s="31"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="33"/>
+      <c r="J12" s="33" t="s">
+        <v>54</v>
+      </c>
       <c r="K12" s="33"/>
       <c r="L12" s="33"/>
       <c r="M12" s="33" t="s">
@@ -3299,7 +3305,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="n">
         <v>152</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="n">
         <v>154</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="n">
         <v>155</v>
       </c>
@@ -3488,7 +3494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27" t="n">
         <v>156</v>
       </c>
@@ -3551,7 +3557,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="n">
         <v>159</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27" t="n">
         <v>160</v>
       </c>
@@ -3677,7 +3683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="27" t="n">
         <v>161</v>
       </c>
@@ -3740,7 +3746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="n">
         <v>162</v>
       </c>
@@ -3781,7 +3787,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27" t="n">
         <v>163</v>
       </c>
@@ -3844,7 +3850,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="n">
         <v>164</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="27" t="n">
         <v>165</v>
       </c>
@@ -3926,7 +3932,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="n">
         <v>166</v>
       </c>
@@ -3967,7 +3973,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="n">
         <v>167</v>
       </c>
@@ -4008,7 +4014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27" t="n">
         <v>168</v>
       </c>
@@ -4049,7 +4055,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="n">
         <v>169</v>
       </c>
@@ -4112,7 +4118,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="n">
         <v>448</v>
       </c>
@@ -4161,7 +4167,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="n">
         <v>449</v>
       </c>
@@ -4204,7 +4210,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="n">
         <v>461</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="n">
         <v>468</v>
       </c>
@@ -4308,7 +4314,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27" t="n">
         <v>475</v>
       </c>
@@ -8591,11 +8597,11 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8655,7 +8661,7 @@
   </sheetPr>
   <dimension ref="A1:G960"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
@@ -8762,7 +8768,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="42" t="s">
         <v>187</v>
       </c>
@@ -8776,7 +8782,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="42" t="s">
         <v>48</v>
       </c>
@@ -8790,7 +8796,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
         <v>192</v>
       </c>
@@ -8804,7 +8810,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="42" t="s">
         <v>195</v>
       </c>
@@ -9805,7 +9811,7 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correzione errori del 12-giugno-2025
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#CAVALLAROXX/CAVALLARO_GIUSEPPE/AUTOFSE/1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#CAVALLAROXX/CAVALLARO_GIUSEPPE/AUTOFSE/1.0/report-checklist.xlsx
@@ -663,13 +663,13 @@
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in modo da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 24" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2025-06-09T11:55:00Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0cdaeaefb66cd7e56cb576724e4b3c0d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.7c02bf2f5b5f72ce9aebf3dec6c0a9b2878f8f5a9239fce7bd9b58e700f8c839.94f2c6e28c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2025-06-16T13:24:00Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9a9ab1cce022075ed268b589fd64073d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.7c02bf2f5b5f72ce9aebf3dec6c0a9b2878f8f5a9239fce7bd9b58e700f8c839.c4ee2ee44b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">OK</t>
@@ -1677,32 +1677,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="285.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="214.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1715,12 +1715,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -2827,11 +2827,11 @@
   <dimension ref="A1:W1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3047,7 +3047,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="15"/>
     </row>
-    <row r="9" s="26" customFormat="true" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="26" customFormat="true" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
         <v>24</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="n">
         <v>32</v>
       </c>
@@ -3181,7 +3181,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="27" t="n">
         <v>40</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="n">
         <v>48</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="27" t="n">
         <v>152</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="n">
         <v>154</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="n">
         <v>155</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="27" t="n">
         <v>156</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="n">
         <v>159</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="27" t="n">
         <v>160</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="27" t="n">
         <v>161</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="27" t="n">
         <v>162</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="27" t="n">
         <v>163</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="27" t="n">
         <v>164</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="27" t="n">
         <v>165</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="27" t="n">
         <v>166</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="27" t="n">
         <v>167</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="27" t="n">
         <v>168</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="27" t="n">
         <v>169</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="27" t="n">
         <v>448</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>137</v>
       </c>
       <c r="F28" s="30" t="n">
-        <v>45817</v>
+        <v>45824</v>
       </c>
       <c r="G28" s="31" t="s">
         <v>138</v>
@@ -4167,7 +4167,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="n">
         <v>449</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="27" t="n">
         <v>461</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="27" t="n">
         <v>468</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="329.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="236.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="27" t="n">
         <v>475</v>
       </c>
@@ -8601,7 +8601,7 @@
       <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -8768,7 +8768,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="42" t="s">
         <v>187</v>
       </c>
@@ -8782,7 +8782,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="42" t="s">
         <v>48</v>
       </c>
@@ -8796,7 +8796,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="42" t="s">
         <v>192</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="42" t="s">
         <v>195</v>
       </c>

</xml_diff>